<commit_message>
updated texas and austin
</commit_message>
<xml_diff>
--- a/AustinCases.xlsx
+++ b/AustinCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mchammas/python-dev/covid/covid19intexas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91864E72-9F60-B040-AECE-BAF8631EC0B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A86CDA6-30EF-BB41-9869-619D98E3042C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="520" windowWidth="28040" windowHeight="16380" xr2:uid="{F8429989-268F-4947-89C6-A2F2A63E1ADA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>sun</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>4/3/20</t>
+  </si>
+  <si>
+    <t>4/4/20</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -772,7 +775,15 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>460</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>

</xml_diff>

<commit_message>
Updated 9/22 except for Dallas
</commit_message>
<xml_diff>
--- a/AustinCases.xlsx
+++ b/AustinCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mchammas/python-dev/covid/covid19intexas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D8F364-5951-4142-A320-103F402AF8B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502FCA22-4E89-574F-97F3-D9441F1AFFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14520" xr2:uid="{F8429989-268F-4947-89C6-A2F2A63E1ADA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="204">
   <si>
     <t>sun</t>
   </si>
@@ -642,6 +642,9 @@
   </si>
   <si>
     <t>9/21/20</t>
+  </si>
+  <si>
+    <t>9/22/20</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5DC3FD-D4C8-3140-B1F4-1B8BC3E1BF59}">
-  <dimension ref="A1:E193"/>
+  <dimension ref="A1:E194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194"/>
+      <selection activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2779,6 +2782,14 @@
         <v>28596</v>
       </c>
     </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B194">
+        <v>28643</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated on 9/27.  Missed a few days
</commit_message>
<xml_diff>
--- a/AustinCases.xlsx
+++ b/AustinCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mchammas/python-dev/covid/covid19intexas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502FCA22-4E89-574F-97F3-D9441F1AFFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F2FFB8-125F-8643-886A-8A4447C11D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14520" xr2:uid="{F8429989-268F-4947-89C6-A2F2A63E1ADA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{F8429989-268F-4947-89C6-A2F2A63E1ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Austin" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="209">
   <si>
     <t>sun</t>
   </si>
@@ -645,6 +645,21 @@
   </si>
   <si>
     <t>9/22/20</t>
+  </si>
+  <si>
+    <t>9/23/20</t>
+  </si>
+  <si>
+    <t>9/24/20</t>
+  </si>
+  <si>
+    <t>9/25/20</t>
+  </si>
+  <si>
+    <t>9/26/20</t>
+  </si>
+  <si>
+    <t>9/27/20</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5DC3FD-D4C8-3140-B1F4-1B8BC3E1BF59}">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2790,6 +2805,46 @@
         <v>28643</v>
       </c>
     </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B195">
+        <v>28745</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B196">
+        <v>28904</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B197">
+        <v>29073</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B198">
+        <v>29130</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B199">
+        <v>29252</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>